<commit_message>
IMP - Quest / A&O
</commit_message>
<xml_diff>
--- a/Quest.xlsx
+++ b/Quest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5481D2AA-BE39-4D5C-836A-7D24C3EF9124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2E62C3CA-4BD0-4922-9611-D1567DBFF964}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{5481D2AA-BE39-4D5C-836A-7D24C3EF9124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE5109C2-6A68-4774-85C2-200B19E05222}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21525" windowHeight="13500" xr2:uid="{5ACD922F-E2B9-468A-8DAF-19A1C97D580A}"/>
+    <workbookView xWindow="6195" yWindow="885" windowWidth="21525" windowHeight="13500" xr2:uid="{5ACD922F-E2B9-468A-8DAF-19A1C97D580A}"/>
   </bookViews>
   <sheets>
     <sheet name="Agito A&amp;O" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>- 開場後退或不動，讓王衝刺的時候比較緊密，SS才有辦法一次兩隻</t>
-  </si>
-  <si>
-    <t>馬爾斯要點</t>
   </si>
   <si>
     <t>- S3 &gt; S4 &gt; (吃衝) &gt; 拉牢 &gt; S1 &gt; 滾去右下 &gt; S2 &gt; S4 &gt; S3 (P1結束)</t>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>- P2切記拉牢，增加穩度 (牢鎖定最遠)</t>
+  </si>
+  <si>
+    <t>馬爾斯要點 / S3由耶、S4副團</t>
   </si>
 </sst>
 </file>
@@ -307,6 +307,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -343,9 +352,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -362,12 +368,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -895,7 +895,7 @@
   <dimension ref="A1:BD54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="AC52" sqref="AC52:BD52"/>
+      <selection activeCell="A50" sqref="A50:AB50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -904,184 +904,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>15</v>
+      <c r="A1" s="14" t="s">
+        <v>14</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="15"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="15"/>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="16"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="15"/>
-      <c r="BD2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="18"/>
+      <c r="AC2" s="18"/>
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="18"/>
+      <c r="AG2" s="18"/>
+      <c r="AH2" s="18"/>
+      <c r="AI2" s="18"/>
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AL2" s="18"/>
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="18"/>
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="18"/>
+      <c r="AV2" s="18"/>
+      <c r="AW2" s="18"/>
+      <c r="AX2" s="18"/>
+      <c r="AY2" s="18"/>
+      <c r="AZ2" s="18"/>
+      <c r="BA2" s="18"/>
+      <c r="BB2" s="18"/>
+      <c r="BC2" s="18"/>
+      <c r="BD2" s="19"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="24"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
-      <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
-      <c r="AJ3" s="24"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24"/>
-      <c r="AN3" s="24"/>
-      <c r="AO3" s="24"/>
-      <c r="AP3" s="24"/>
-      <c r="AQ3" s="24"/>
-      <c r="AR3" s="24"/>
-      <c r="AS3" s="24"/>
-      <c r="AT3" s="24"/>
-      <c r="AU3" s="24"/>
-      <c r="AV3" s="24"/>
-      <c r="AW3" s="24"/>
-      <c r="AX3" s="24"/>
-      <c r="AY3" s="24"/>
-      <c r="AZ3" s="24"/>
-      <c r="BA3" s="24"/>
-      <c r="BB3" s="24"/>
-      <c r="BC3" s="24"/>
-      <c r="BD3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="26"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="26"/>
+      <c r="AE3" s="26"/>
+      <c r="AF3" s="26"/>
+      <c r="AG3" s="26"/>
+      <c r="AH3" s="26"/>
+      <c r="AI3" s="26"/>
+      <c r="AJ3" s="26"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="26"/>
+      <c r="AM3" s="26"/>
+      <c r="AN3" s="26"/>
+      <c r="AO3" s="26"/>
+      <c r="AP3" s="26"/>
+      <c r="AQ3" s="26"/>
+      <c r="AR3" s="26"/>
+      <c r="AS3" s="26"/>
+      <c r="AT3" s="26"/>
+      <c r="AU3" s="26"/>
+      <c r="AV3" s="26"/>
+      <c r="AW3" s="26"/>
+      <c r="AX3" s="26"/>
+      <c r="AY3" s="26"/>
+      <c r="AZ3" s="26"/>
+      <c r="BA3" s="26"/>
+      <c r="BB3" s="26"/>
+      <c r="BC3" s="26"/>
+      <c r="BD3" s="27"/>
     </row>
     <row r="4" spans="1:56" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -2302,184 +2302,184 @@
       <c r="BD24" s="4"/>
     </row>
     <row r="25" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="21"/>
-      <c r="V25" s="21"/>
-      <c r="W25" s="21"/>
-      <c r="X25" s="21"/>
-      <c r="Y25" s="21"/>
-      <c r="Z25" s="21"/>
-      <c r="AA25" s="21"/>
-      <c r="AB25" s="21"/>
-      <c r="AC25" s="21"/>
-      <c r="AD25" s="21"/>
-      <c r="AE25" s="21"/>
-      <c r="AF25" s="21"/>
-      <c r="AG25" s="21"/>
-      <c r="AH25" s="21"/>
-      <c r="AI25" s="21"/>
-      <c r="AJ25" s="21"/>
-      <c r="AK25" s="21"/>
-      <c r="AL25" s="21"/>
-      <c r="AM25" s="21"/>
-      <c r="AN25" s="21"/>
-      <c r="AO25" s="21"/>
-      <c r="AP25" s="21"/>
-      <c r="AQ25" s="21"/>
-      <c r="AR25" s="21"/>
-      <c r="AS25" s="21"/>
-      <c r="AT25" s="21"/>
-      <c r="AU25" s="21"/>
-      <c r="AV25" s="21"/>
-      <c r="AW25" s="21"/>
-      <c r="AX25" s="21"/>
-      <c r="AY25" s="21"/>
-      <c r="AZ25" s="21"/>
-      <c r="BA25" s="21"/>
-      <c r="BB25" s="21"/>
-      <c r="BC25" s="21"/>
-      <c r="BD25" s="22"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
+      <c r="Z25" s="24"/>
+      <c r="AA25" s="24"/>
+      <c r="AB25" s="24"/>
+      <c r="AC25" s="24"/>
+      <c r="AD25" s="24"/>
+      <c r="AE25" s="24"/>
+      <c r="AF25" s="24"/>
+      <c r="AG25" s="24"/>
+      <c r="AH25" s="24"/>
+      <c r="AI25" s="24"/>
+      <c r="AJ25" s="24"/>
+      <c r="AK25" s="24"/>
+      <c r="AL25" s="24"/>
+      <c r="AM25" s="24"/>
+      <c r="AN25" s="24"/>
+      <c r="AO25" s="24"/>
+      <c r="AP25" s="24"/>
+      <c r="AQ25" s="24"/>
+      <c r="AR25" s="24"/>
+      <c r="AS25" s="24"/>
+      <c r="AT25" s="24"/>
+      <c r="AU25" s="24"/>
+      <c r="AV25" s="24"/>
+      <c r="AW25" s="24"/>
+      <c r="AX25" s="24"/>
+      <c r="AY25" s="24"/>
+      <c r="AZ25" s="24"/>
+      <c r="BA25" s="24"/>
+      <c r="BB25" s="24"/>
+      <c r="BC25" s="24"/>
+      <c r="BD25" s="25"/>
     </row>
     <row r="26" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
-      <c r="AD26" s="30"/>
-      <c r="AE26" s="30"/>
-      <c r="AF26" s="30"/>
-      <c r="AG26" s="30"/>
-      <c r="AH26" s="30"/>
-      <c r="AI26" s="30"/>
-      <c r="AJ26" s="30"/>
-      <c r="AK26" s="30"/>
-      <c r="AL26" s="30"/>
-      <c r="AM26" s="30"/>
-      <c r="AN26" s="30"/>
-      <c r="AO26" s="30"/>
-      <c r="AP26" s="30"/>
-      <c r="AQ26" s="30"/>
-      <c r="AR26" s="30"/>
-      <c r="AS26" s="30"/>
-      <c r="AT26" s="30"/>
-      <c r="AU26" s="30"/>
-      <c r="AV26" s="30"/>
-      <c r="AW26" s="30"/>
-      <c r="AX26" s="30"/>
-      <c r="AY26" s="30"/>
-      <c r="AZ26" s="30"/>
-      <c r="BA26" s="30"/>
-      <c r="BB26" s="30"/>
-      <c r="BC26" s="30"/>
-      <c r="BD26" s="31"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="12"/>
+      <c r="AJ26" s="12"/>
+      <c r="AK26" s="12"/>
+      <c r="AL26" s="12"/>
+      <c r="AM26" s="12"/>
+      <c r="AN26" s="12"/>
+      <c r="AO26" s="12"/>
+      <c r="AP26" s="12"/>
+      <c r="AQ26" s="12"/>
+      <c r="AR26" s="12"/>
+      <c r="AS26" s="12"/>
+      <c r="AT26" s="12"/>
+      <c r="AU26" s="12"/>
+      <c r="AV26" s="12"/>
+      <c r="AW26" s="12"/>
+      <c r="AX26" s="12"/>
+      <c r="AY26" s="12"/>
+      <c r="AZ26" s="12"/>
+      <c r="BA26" s="12"/>
+      <c r="BB26" s="12"/>
+      <c r="BC26" s="12"/>
+      <c r="BD26" s="13"/>
     </row>
     <row r="27" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="30"/>
-      <c r="AE27" s="30"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="30"/>
-      <c r="AI27" s="30"/>
-      <c r="AJ27" s="30"/>
-      <c r="AK27" s="30"/>
-      <c r="AL27" s="30"/>
-      <c r="AM27" s="30"/>
-      <c r="AN27" s="30"/>
-      <c r="AO27" s="30"/>
-      <c r="AP27" s="30"/>
-      <c r="AQ27" s="30"/>
-      <c r="AR27" s="30"/>
-      <c r="AS27" s="30"/>
-      <c r="AT27" s="30"/>
-      <c r="AU27" s="30"/>
-      <c r="AV27" s="30"/>
-      <c r="AW27" s="30"/>
-      <c r="AX27" s="30"/>
-      <c r="AY27" s="30"/>
-      <c r="AZ27" s="30"/>
-      <c r="BA27" s="30"/>
-      <c r="BB27" s="30"/>
-      <c r="BC27" s="30"/>
-      <c r="BD27" s="31"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="12"/>
+      <c r="AF27" s="12"/>
+      <c r="AG27" s="12"/>
+      <c r="AH27" s="12"/>
+      <c r="AI27" s="12"/>
+      <c r="AJ27" s="12"/>
+      <c r="AK27" s="12"/>
+      <c r="AL27" s="12"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="12"/>
+      <c r="AQ27" s="12"/>
+      <c r="AR27" s="12"/>
+      <c r="AS27" s="12"/>
+      <c r="AT27" s="12"/>
+      <c r="AU27" s="12"/>
+      <c r="AV27" s="12"/>
+      <c r="AW27" s="12"/>
+      <c r="AX27" s="12"/>
+      <c r="AY27" s="12"/>
+      <c r="AZ27" s="12"/>
+      <c r="BA27" s="12"/>
+      <c r="BB27" s="12"/>
+      <c r="BC27" s="12"/>
+      <c r="BD27" s="13"/>
     </row>
     <row r="28" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
@@ -3700,377 +3700,378 @@
       <c r="BD48" s="10"/>
     </row>
     <row r="49" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="24"/>
+      <c r="S49" s="24"/>
+      <c r="T49" s="24"/>
+      <c r="U49" s="24"/>
+      <c r="V49" s="24"/>
+      <c r="W49" s="24"/>
+      <c r="X49" s="24"/>
+      <c r="Y49" s="24"/>
+      <c r="Z49" s="24"/>
+      <c r="AA49" s="24"/>
+      <c r="AB49" s="25"/>
+      <c r="AC49" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD49" s="24"/>
+      <c r="AE49" s="24"/>
+      <c r="AF49" s="24"/>
+      <c r="AG49" s="24"/>
+      <c r="AH49" s="24"/>
+      <c r="AI49" s="24"/>
+      <c r="AJ49" s="24"/>
+      <c r="AK49" s="24"/>
+      <c r="AL49" s="24"/>
+      <c r="AM49" s="24"/>
+      <c r="AN49" s="24"/>
+      <c r="AO49" s="24"/>
+      <c r="AP49" s="24"/>
+      <c r="AQ49" s="24"/>
+      <c r="AR49" s="24"/>
+      <c r="AS49" s="24"/>
+      <c r="AT49" s="24"/>
+      <c r="AU49" s="24"/>
+      <c r="AV49" s="24"/>
+      <c r="AW49" s="24"/>
+      <c r="AX49" s="24"/>
+      <c r="AY49" s="24"/>
+      <c r="AZ49" s="24"/>
+      <c r="BA49" s="24"/>
+      <c r="BB49" s="24"/>
+      <c r="BC49" s="24"/>
+      <c r="BD49" s="25"/>
+    </row>
+    <row r="50" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
-      <c r="P49" s="21"/>
-      <c r="Q49" s="21"/>
-      <c r="R49" s="21"/>
-      <c r="S49" s="21"/>
-      <c r="T49" s="21"/>
-      <c r="U49" s="21"/>
-      <c r="V49" s="21"/>
-      <c r="W49" s="21"/>
-      <c r="X49" s="21"/>
-      <c r="Y49" s="21"/>
-      <c r="Z49" s="21"/>
-      <c r="AA49" s="21"/>
-      <c r="AB49" s="22"/>
-      <c r="AC49" s="20" t="s">
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+      <c r="L50" s="26"/>
+      <c r="M50" s="26"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="26"/>
+      <c r="P50" s="26"/>
+      <c r="Q50" s="26"/>
+      <c r="R50" s="26"/>
+      <c r="S50" s="26"/>
+      <c r="T50" s="26"/>
+      <c r="U50" s="26"/>
+      <c r="V50" s="26"/>
+      <c r="W50" s="26"/>
+      <c r="X50" s="26"/>
+      <c r="Y50" s="26"/>
+      <c r="Z50" s="26"/>
+      <c r="AA50" s="26"/>
+      <c r="AB50" s="27"/>
+      <c r="AC50" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AD49" s="21"/>
-      <c r="AE49" s="21"/>
-      <c r="AF49" s="21"/>
-      <c r="AG49" s="21"/>
-      <c r="AH49" s="21"/>
-      <c r="AI49" s="21"/>
-      <c r="AJ49" s="21"/>
-      <c r="AK49" s="21"/>
-      <c r="AL49" s="21"/>
-      <c r="AM49" s="21"/>
-      <c r="AN49" s="21"/>
-      <c r="AO49" s="21"/>
-      <c r="AP49" s="21"/>
-      <c r="AQ49" s="21"/>
-      <c r="AR49" s="21"/>
-      <c r="AS49" s="21"/>
-      <c r="AT49" s="21"/>
-      <c r="AU49" s="21"/>
-      <c r="AV49" s="21"/>
-      <c r="AW49" s="21"/>
-      <c r="AX49" s="21"/>
-      <c r="AY49" s="21"/>
-      <c r="AZ49" s="21"/>
-      <c r="BA49" s="21"/>
-      <c r="BB49" s="21"/>
-      <c r="BC49" s="21"/>
-      <c r="BD49" s="22"/>
-    </row>
-    <row r="50" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="AD50" s="26"/>
+      <c r="AE50" s="26"/>
+      <c r="AF50" s="26"/>
+      <c r="AG50" s="26"/>
+      <c r="AH50" s="26"/>
+      <c r="AI50" s="26"/>
+      <c r="AJ50" s="26"/>
+      <c r="AK50" s="26"/>
+      <c r="AL50" s="26"/>
+      <c r="AM50" s="26"/>
+      <c r="AN50" s="26"/>
+      <c r="AO50" s="26"/>
+      <c r="AP50" s="26"/>
+      <c r="AQ50" s="26"/>
+      <c r="AR50" s="26"/>
+      <c r="AS50" s="26"/>
+      <c r="AT50" s="26"/>
+      <c r="AU50" s="26"/>
+      <c r="AV50" s="26"/>
+      <c r="AW50" s="26"/>
+      <c r="AX50" s="26"/>
+      <c r="AY50" s="26"/>
+      <c r="AZ50" s="26"/>
+      <c r="BA50" s="26"/>
+      <c r="BB50" s="26"/>
+      <c r="BC50" s="26"/>
+      <c r="BD50" s="27"/>
+    </row>
+    <row r="51" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24"/>
-      <c r="K50" s="24"/>
-      <c r="L50" s="24"/>
-      <c r="M50" s="24"/>
-      <c r="N50" s="24"/>
-      <c r="O50" s="24"/>
-      <c r="P50" s="24"/>
-      <c r="Q50" s="24"/>
-      <c r="R50" s="24"/>
-      <c r="S50" s="24"/>
-      <c r="T50" s="24"/>
-      <c r="U50" s="24"/>
-      <c r="V50" s="24"/>
-      <c r="W50" s="24"/>
-      <c r="X50" s="24"/>
-      <c r="Y50" s="24"/>
-      <c r="Z50" s="24"/>
-      <c r="AA50" s="24"/>
-      <c r="AB50" s="25"/>
-      <c r="AC50" s="23" t="s">
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="26"/>
+      <c r="P51" s="26"/>
+      <c r="Q51" s="26"/>
+      <c r="R51" s="26"/>
+      <c r="S51" s="26"/>
+      <c r="T51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="V51" s="26"/>
+      <c r="W51" s="26"/>
+      <c r="X51" s="26"/>
+      <c r="Y51" s="26"/>
+      <c r="Z51" s="26"/>
+      <c r="AA51" s="26"/>
+      <c r="AB51" s="27"/>
+      <c r="AC51" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AD50" s="24"/>
-      <c r="AE50" s="24"/>
-      <c r="AF50" s="24"/>
-      <c r="AG50" s="24"/>
-      <c r="AH50" s="24"/>
-      <c r="AI50" s="24"/>
-      <c r="AJ50" s="24"/>
-      <c r="AK50" s="24"/>
-      <c r="AL50" s="24"/>
-      <c r="AM50" s="24"/>
-      <c r="AN50" s="24"/>
-      <c r="AO50" s="24"/>
-      <c r="AP50" s="24"/>
-      <c r="AQ50" s="24"/>
-      <c r="AR50" s="24"/>
-      <c r="AS50" s="24"/>
-      <c r="AT50" s="24"/>
-      <c r="AU50" s="24"/>
-      <c r="AV50" s="24"/>
-      <c r="AW50" s="24"/>
-      <c r="AX50" s="24"/>
-      <c r="AY50" s="24"/>
-      <c r="AZ50" s="24"/>
-      <c r="BA50" s="24"/>
-      <c r="BB50" s="24"/>
-      <c r="BC50" s="24"/>
-      <c r="BD50" s="25"/>
-    </row>
-    <row r="51" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
+      <c r="AD51" s="26"/>
+      <c r="AE51" s="26"/>
+      <c r="AF51" s="26"/>
+      <c r="AG51" s="26"/>
+      <c r="AH51" s="26"/>
+      <c r="AI51" s="26"/>
+      <c r="AJ51" s="26"/>
+      <c r="AK51" s="26"/>
+      <c r="AL51" s="26"/>
+      <c r="AM51" s="26"/>
+      <c r="AN51" s="26"/>
+      <c r="AO51" s="26"/>
+      <c r="AP51" s="26"/>
+      <c r="AQ51" s="26"/>
+      <c r="AR51" s="26"/>
+      <c r="AS51" s="26"/>
+      <c r="AT51" s="26"/>
+      <c r="AU51" s="26"/>
+      <c r="AV51" s="26"/>
+      <c r="AW51" s="26"/>
+      <c r="AX51" s="26"/>
+      <c r="AY51" s="26"/>
+      <c r="AZ51" s="26"/>
+      <c r="BA51" s="26"/>
+      <c r="BB51" s="26"/>
+      <c r="BC51" s="26"/>
+      <c r="BD51" s="27"/>
+    </row>
+    <row r="52" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="24"/>
-      <c r="S51" s="24"/>
-      <c r="T51" s="24"/>
-      <c r="U51" s="24"/>
-      <c r="V51" s="24"/>
-      <c r="W51" s="24"/>
-      <c r="X51" s="24"/>
-      <c r="Y51" s="24"/>
-      <c r="Z51" s="24"/>
-      <c r="AA51" s="24"/>
-      <c r="AB51" s="25"/>
-      <c r="AC51" s="23" t="s">
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+      <c r="O52" s="29"/>
+      <c r="P52" s="29"/>
+      <c r="Q52" s="29"/>
+      <c r="R52" s="29"/>
+      <c r="S52" s="29"/>
+      <c r="T52" s="29"/>
+      <c r="U52" s="29"/>
+      <c r="V52" s="29"/>
+      <c r="W52" s="29"/>
+      <c r="X52" s="29"/>
+      <c r="Y52" s="29"/>
+      <c r="Z52" s="29"/>
+      <c r="AA52" s="29"/>
+      <c r="AB52" s="30"/>
+      <c r="AC52" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD52" s="29"/>
+      <c r="AE52" s="29"/>
+      <c r="AF52" s="29"/>
+      <c r="AG52" s="29"/>
+      <c r="AH52" s="29"/>
+      <c r="AI52" s="29"/>
+      <c r="AJ52" s="29"/>
+      <c r="AK52" s="29"/>
+      <c r="AL52" s="29"/>
+      <c r="AM52" s="29"/>
+      <c r="AN52" s="29"/>
+      <c r="AO52" s="29"/>
+      <c r="AP52" s="29"/>
+      <c r="AQ52" s="29"/>
+      <c r="AR52" s="29"/>
+      <c r="AS52" s="29"/>
+      <c r="AT52" s="29"/>
+      <c r="AU52" s="29"/>
+      <c r="AV52" s="29"/>
+      <c r="AW52" s="29"/>
+      <c r="AX52" s="29"/>
+      <c r="AY52" s="29"/>
+      <c r="AZ52" s="29"/>
+      <c r="BA52" s="29"/>
+      <c r="BB52" s="29"/>
+      <c r="BC52" s="29"/>
+      <c r="BD52" s="30"/>
+    </row>
+    <row r="53" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="AD51" s="24"/>
-      <c r="AE51" s="24"/>
-      <c r="AF51" s="24"/>
-      <c r="AG51" s="24"/>
-      <c r="AH51" s="24"/>
-      <c r="AI51" s="24"/>
-      <c r="AJ51" s="24"/>
-      <c r="AK51" s="24"/>
-      <c r="AL51" s="24"/>
-      <c r="AM51" s="24"/>
-      <c r="AN51" s="24"/>
-      <c r="AO51" s="24"/>
-      <c r="AP51" s="24"/>
-      <c r="AQ51" s="24"/>
-      <c r="AR51" s="24"/>
-      <c r="AS51" s="24"/>
-      <c r="AT51" s="24"/>
-      <c r="AU51" s="24"/>
-      <c r="AV51" s="24"/>
-      <c r="AW51" s="24"/>
-      <c r="AX51" s="24"/>
-      <c r="AY51" s="24"/>
-      <c r="AZ51" s="24"/>
-      <c r="BA51" s="24"/>
-      <c r="BB51" s="24"/>
-      <c r="BC51" s="24"/>
-      <c r="BD51" s="25"/>
-    </row>
-    <row r="52" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
-      <c r="M52" s="27"/>
-      <c r="N52" s="27"/>
-      <c r="O52" s="27"/>
-      <c r="P52" s="27"/>
-      <c r="Q52" s="27"/>
-      <c r="R52" s="27"/>
-      <c r="S52" s="27"/>
-      <c r="T52" s="27"/>
-      <c r="U52" s="27"/>
-      <c r="V52" s="27"/>
-      <c r="W52" s="27"/>
-      <c r="X52" s="27"/>
-      <c r="Y52" s="27"/>
-      <c r="Z52" s="27"/>
-      <c r="AA52" s="27"/>
-      <c r="AB52" s="28"/>
-      <c r="AC52" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD52" s="27"/>
-      <c r="AE52" s="27"/>
-      <c r="AF52" s="27"/>
-      <c r="AG52" s="27"/>
-      <c r="AH52" s="27"/>
-      <c r="AI52" s="27"/>
-      <c r="AJ52" s="27"/>
-      <c r="AK52" s="27"/>
-      <c r="AL52" s="27"/>
-      <c r="AM52" s="27"/>
-      <c r="AN52" s="27"/>
-      <c r="AO52" s="27"/>
-      <c r="AP52" s="27"/>
-      <c r="AQ52" s="27"/>
-      <c r="AR52" s="27"/>
-      <c r="AS52" s="27"/>
-      <c r="AT52" s="27"/>
-      <c r="AU52" s="27"/>
-      <c r="AV52" s="27"/>
-      <c r="AW52" s="27"/>
-      <c r="AX52" s="27"/>
-      <c r="AY52" s="27"/>
-      <c r="AZ52" s="27"/>
-      <c r="BA52" s="27"/>
-      <c r="BB52" s="27"/>
-      <c r="BC52" s="27"/>
-      <c r="BD52" s="28"/>
-    </row>
-    <row r="53" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="18"/>
+      <c r="U53" s="18"/>
+      <c r="V53" s="18"/>
+      <c r="W53" s="18"/>
+      <c r="X53" s="18"/>
+      <c r="Y53" s="18"/>
+      <c r="Z53" s="18"/>
+      <c r="AA53" s="18"/>
+      <c r="AB53" s="18"/>
+      <c r="AC53" s="18"/>
+      <c r="AD53" s="18"/>
+      <c r="AE53" s="18"/>
+      <c r="AF53" s="18"/>
+      <c r="AG53" s="18"/>
+      <c r="AH53" s="18"/>
+      <c r="AI53" s="18"/>
+      <c r="AJ53" s="18"/>
+      <c r="AK53" s="18"/>
+      <c r="AL53" s="18"/>
+      <c r="AM53" s="18"/>
+      <c r="AN53" s="18"/>
+      <c r="AO53" s="18"/>
+      <c r="AP53" s="18"/>
+      <c r="AQ53" s="18"/>
+      <c r="AR53" s="18"/>
+      <c r="AS53" s="18"/>
+      <c r="AT53" s="18"/>
+      <c r="AU53" s="18"/>
+      <c r="AV53" s="18"/>
+      <c r="AW53" s="18"/>
+      <c r="AX53" s="18"/>
+      <c r="AY53" s="18"/>
+      <c r="AZ53" s="18"/>
+      <c r="BA53" s="18"/>
+      <c r="BB53" s="18"/>
+      <c r="BC53" s="18"/>
+      <c r="BD53" s="19"/>
+    </row>
+    <row r="54" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="15"/>
-      <c r="U53" s="15"/>
-      <c r="V53" s="15"/>
-      <c r="W53" s="15"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="15"/>
-      <c r="Z53" s="15"/>
-      <c r="AA53" s="15"/>
-      <c r="AB53" s="15"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="15"/>
-      <c r="AE53" s="15"/>
-      <c r="AF53" s="15"/>
-      <c r="AG53" s="15"/>
-      <c r="AH53" s="15"/>
-      <c r="AI53" s="15"/>
-      <c r="AJ53" s="15"/>
-      <c r="AK53" s="15"/>
-      <c r="AL53" s="15"/>
-      <c r="AM53" s="15"/>
-      <c r="AN53" s="15"/>
-      <c r="AO53" s="15"/>
-      <c r="AP53" s="15"/>
-      <c r="AQ53" s="15"/>
-      <c r="AR53" s="15"/>
-      <c r="AS53" s="15"/>
-      <c r="AT53" s="15"/>
-      <c r="AU53" s="15"/>
-      <c r="AV53" s="15"/>
-      <c r="AW53" s="15"/>
-      <c r="AX53" s="15"/>
-      <c r="AY53" s="15"/>
-      <c r="AZ53" s="15"/>
-      <c r="BA53" s="15"/>
-      <c r="BB53" s="15"/>
-      <c r="BC53" s="15"/>
-      <c r="BD53" s="16"/>
-    </row>
-    <row r="54" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="21"/>
+      <c r="P54" s="21"/>
+      <c r="Q54" s="21"/>
+      <c r="R54" s="21"/>
+      <c r="S54" s="21"/>
+      <c r="T54" s="21"/>
+      <c r="U54" s="21"/>
+      <c r="V54" s="21"/>
+      <c r="W54" s="21"/>
+      <c r="X54" s="21"/>
+      <c r="Y54" s="21"/>
+      <c r="Z54" s="21"/>
+      <c r="AA54" s="21"/>
+      <c r="AB54" s="21"/>
+      <c r="AC54" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="18"/>
-      <c r="U54" s="18"/>
-      <c r="V54" s="18"/>
-      <c r="W54" s="18"/>
-      <c r="X54" s="18"/>
-      <c r="Y54" s="18"/>
-      <c r="Z54" s="18"/>
-      <c r="AA54" s="18"/>
-      <c r="AB54" s="18"/>
-      <c r="AC54" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD54" s="18"/>
-      <c r="AE54" s="18"/>
-      <c r="AF54" s="18"/>
-      <c r="AG54" s="18"/>
-      <c r="AH54" s="18"/>
-      <c r="AI54" s="18"/>
-      <c r="AJ54" s="18"/>
-      <c r="AK54" s="18"/>
-      <c r="AL54" s="18"/>
-      <c r="AM54" s="18"/>
-      <c r="AN54" s="18"/>
-      <c r="AO54" s="18"/>
-      <c r="AP54" s="18"/>
-      <c r="AQ54" s="18"/>
-      <c r="AR54" s="18"/>
-      <c r="AS54" s="18"/>
-      <c r="AT54" s="18"/>
-      <c r="AU54" s="18"/>
-      <c r="AV54" s="18"/>
-      <c r="AW54" s="18"/>
-      <c r="AX54" s="18"/>
-      <c r="AY54" s="18"/>
-      <c r="AZ54" s="18"/>
-      <c r="BA54" s="18"/>
-      <c r="BB54" s="18"/>
-      <c r="BC54" s="18"/>
-      <c r="BD54" s="19"/>
+      <c r="AD54" s="21"/>
+      <c r="AE54" s="21"/>
+      <c r="AF54" s="21"/>
+      <c r="AG54" s="21"/>
+      <c r="AH54" s="21"/>
+      <c r="AI54" s="21"/>
+      <c r="AJ54" s="21"/>
+      <c r="AK54" s="21"/>
+      <c r="AL54" s="21"/>
+      <c r="AM54" s="21"/>
+      <c r="AN54" s="21"/>
+      <c r="AO54" s="21"/>
+      <c r="AP54" s="21"/>
+      <c r="AQ54" s="21"/>
+      <c r="AR54" s="21"/>
+      <c r="AS54" s="21"/>
+      <c r="AT54" s="21"/>
+      <c r="AU54" s="21"/>
+      <c r="AV54" s="21"/>
+      <c r="AW54" s="21"/>
+      <c r="AX54" s="21"/>
+      <c r="AY54" s="21"/>
+      <c r="AZ54" s="21"/>
+      <c r="BA54" s="21"/>
+      <c r="BB54" s="21"/>
+      <c r="BC54" s="21"/>
+      <c r="BD54" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A26:BD26"/>
     <mergeCell ref="A27:BD27"/>
     <mergeCell ref="A1:BD1"/>
     <mergeCell ref="A53:BD53"/>
@@ -4087,7 +4088,6 @@
     <mergeCell ref="A50:AB50"/>
     <mergeCell ref="A51:AB51"/>
     <mergeCell ref="A52:AB52"/>
-    <mergeCell ref="A26:BD26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
IMP - Main xlsx
</commit_message>
<xml_diff>
--- a/Quest.xlsx
+++ b/Quest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{5481D2AA-BE39-4D5C-836A-7D24C3EF9124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{15851184-AA55-43E4-B3F4-0AC8A42B2272}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{5481D2AA-BE39-4D5C-836A-7D24C3EF9124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08AF62C7-0D7C-4312-B1B3-78F0217147E8}"/>
   <bookViews>
-    <workbookView xWindow="33795" yWindow="2010" windowWidth="20190" windowHeight="13560" xr2:uid="{5ACD922F-E2B9-468A-8DAF-19A1C97D580A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24585" windowHeight="15765" xr2:uid="{5ACD922F-E2B9-468A-8DAF-19A1C97D580A}"/>
   </bookViews>
   <sheets>
     <sheet name="Agito A&amp;O" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>- P2: 紫圈變龍 &gt; 拉牢 &gt; (王靠中) &gt; S1 &gt; FS &gt; S3 &gt; S4</t>
   </si>
   <si>
-    <t>影片參考: https://youtu.be/2vLxB4hdzao</t>
-  </si>
-  <si>
     <t>打法大量參考NGA上第一種速刷法</t>
   </si>
   <si>
@@ -87,6 +84,53 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">影片參考: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://youtu.be/2vLxB4hdzao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (馬24+3葉) </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://youtu.be/CxLXB2hwYqU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (馬24 + 德菲)</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="18"/>
         <color rgb="FFFF0000"/>
@@ -104,7 +148,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Oasis of the Maniacs - 2020/06/26 2:51 PM CDT</t>
+      <t xml:space="preserve"> Oasis of the Maniacs - 2020/06/26 10:52 PM CDT</t>
     </r>
   </si>
 </sst>
@@ -112,7 +156,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +174,14 @@
     <font>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,43 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -364,6 +380,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,6 +397,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,8 +949,8 @@
   </sheetPr>
   <dimension ref="A1:BD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:BD1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:BD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -907,184 +959,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="27"/>
-      <c r="AX1" s="27"/>
-      <c r="AY1" s="27"/>
-      <c r="AZ1" s="27"/>
-      <c r="BA1" s="27"/>
-      <c r="BB1" s="27"/>
-      <c r="BC1" s="27"/>
-      <c r="BD1" s="28"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="15"/>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="15"/>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="16"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30"/>
-      <c r="AO2" s="30"/>
-      <c r="AP2" s="30"/>
-      <c r="AQ2" s="30"/>
-      <c r="AR2" s="30"/>
-      <c r="AS2" s="30"/>
-      <c r="AT2" s="30"/>
-      <c r="AU2" s="30"/>
-      <c r="AV2" s="30"/>
-      <c r="AW2" s="30"/>
-      <c r="AX2" s="30"/>
-      <c r="AY2" s="30"/>
-      <c r="AZ2" s="30"/>
-      <c r="BA2" s="30"/>
-      <c r="BB2" s="30"/>
-      <c r="BC2" s="30"/>
-      <c r="BD2" s="31"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="21"/>
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="21"/>
+      <c r="AE2" s="21"/>
+      <c r="AF2" s="21"/>
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="21"/>
+      <c r="AL2" s="21"/>
+      <c r="AM2" s="21"/>
+      <c r="AN2" s="21"/>
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="21"/>
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="21"/>
+      <c r="AT2" s="21"/>
+      <c r="AU2" s="21"/>
+      <c r="AV2" s="21"/>
+      <c r="AW2" s="21"/>
+      <c r="AX2" s="21"/>
+      <c r="AY2" s="21"/>
+      <c r="AZ2" s="21"/>
+      <c r="BA2" s="21"/>
+      <c r="BB2" s="21"/>
+      <c r="BC2" s="21"/>
+      <c r="BD2" s="22"/>
     </row>
     <row r="3" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="18"/>
-      <c r="AA3" s="18"/>
-      <c r="AB3" s="18"/>
-      <c r="AC3" s="18"/>
-      <c r="AD3" s="18"/>
-      <c r="AE3" s="18"/>
-      <c r="AF3" s="18"/>
-      <c r="AG3" s="18"/>
-      <c r="AH3" s="18"/>
-      <c r="AI3" s="18"/>
-      <c r="AJ3" s="18"/>
-      <c r="AK3" s="18"/>
-      <c r="AL3" s="18"/>
-      <c r="AM3" s="18"/>
-      <c r="AN3" s="18"/>
-      <c r="AO3" s="18"/>
-      <c r="AP3" s="18"/>
-      <c r="AQ3" s="18"/>
-      <c r="AR3" s="18"/>
-      <c r="AS3" s="18"/>
-      <c r="AT3" s="18"/>
-      <c r="AU3" s="18"/>
-      <c r="AV3" s="18"/>
-      <c r="AW3" s="18"/>
-      <c r="AX3" s="18"/>
-      <c r="AY3" s="18"/>
-      <c r="AZ3" s="18"/>
-      <c r="BA3" s="18"/>
-      <c r="BB3" s="18"/>
-      <c r="BC3" s="18"/>
-      <c r="BD3" s="19"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="23"/>
+      <c r="AH3" s="23"/>
+      <c r="AI3" s="23"/>
+      <c r="AJ3" s="23"/>
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="24"/>
     </row>
     <row r="4" spans="1:56" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -2305,184 +2357,184 @@
       <c r="BD24" s="4"/>
     </row>
     <row r="25" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
-      <c r="AA25" s="15"/>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" s="15"/>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="15"/>
-      <c r="AG25" s="15"/>
-      <c r="AH25" s="15"/>
-      <c r="AI25" s="15"/>
-      <c r="AJ25" s="15"/>
-      <c r="AK25" s="15"/>
-      <c r="AL25" s="15"/>
-      <c r="AM25" s="15"/>
-      <c r="AN25" s="15"/>
-      <c r="AO25" s="15"/>
-      <c r="AP25" s="15"/>
-      <c r="AQ25" s="15"/>
-      <c r="AR25" s="15"/>
-      <c r="AS25" s="15"/>
-      <c r="AT25" s="15"/>
-      <c r="AU25" s="15"/>
-      <c r="AV25" s="15"/>
-      <c r="AW25" s="15"/>
-      <c r="AX25" s="15"/>
-      <c r="AY25" s="15"/>
-      <c r="AZ25" s="15"/>
-      <c r="BA25" s="15"/>
-      <c r="BB25" s="15"/>
-      <c r="BC25" s="15"/>
-      <c r="BD25" s="16"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="18"/>
+      <c r="U25" s="18"/>
+      <c r="V25" s="18"/>
+      <c r="W25" s="18"/>
+      <c r="X25" s="18"/>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="18"/>
+      <c r="AB25" s="18"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="18"/>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="18"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+      <c r="AL25" s="18"/>
+      <c r="AM25" s="18"/>
+      <c r="AN25" s="18"/>
+      <c r="AO25" s="18"/>
+      <c r="AP25" s="18"/>
+      <c r="AQ25" s="18"/>
+      <c r="AR25" s="18"/>
+      <c r="AS25" s="18"/>
+      <c r="AT25" s="18"/>
+      <c r="AU25" s="18"/>
+      <c r="AV25" s="18"/>
+      <c r="AW25" s="18"/>
+      <c r="AX25" s="18"/>
+      <c r="AY25" s="18"/>
+      <c r="AZ25" s="18"/>
+      <c r="BA25" s="18"/>
+      <c r="BB25" s="18"/>
+      <c r="BC25" s="18"/>
+      <c r="BD25" s="19"/>
     </row>
     <row r="26" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="24"/>
-      <c r="AA26" s="24"/>
-      <c r="AB26" s="24"/>
-      <c r="AC26" s="24"/>
-      <c r="AD26" s="24"/>
-      <c r="AE26" s="24"/>
-      <c r="AF26" s="24"/>
-      <c r="AG26" s="24"/>
-      <c r="AH26" s="24"/>
-      <c r="AI26" s="24"/>
-      <c r="AJ26" s="24"/>
-      <c r="AK26" s="24"/>
-      <c r="AL26" s="24"/>
-      <c r="AM26" s="24"/>
-      <c r="AN26" s="24"/>
-      <c r="AO26" s="24"/>
-      <c r="AP26" s="24"/>
-      <c r="AQ26" s="24"/>
-      <c r="AR26" s="24"/>
-      <c r="AS26" s="24"/>
-      <c r="AT26" s="24"/>
-      <c r="AU26" s="24"/>
-      <c r="AV26" s="24"/>
-      <c r="AW26" s="24"/>
-      <c r="AX26" s="24"/>
-      <c r="AY26" s="24"/>
-      <c r="AZ26" s="24"/>
-      <c r="BA26" s="24"/>
-      <c r="BB26" s="24"/>
-      <c r="BC26" s="24"/>
-      <c r="BD26" s="25"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="12"/>
+      <c r="AE26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AH26" s="12"/>
+      <c r="AI26" s="12"/>
+      <c r="AJ26" s="12"/>
+      <c r="AK26" s="12"/>
+      <c r="AL26" s="12"/>
+      <c r="AM26" s="12"/>
+      <c r="AN26" s="12"/>
+      <c r="AO26" s="12"/>
+      <c r="AP26" s="12"/>
+      <c r="AQ26" s="12"/>
+      <c r="AR26" s="12"/>
+      <c r="AS26" s="12"/>
+      <c r="AT26" s="12"/>
+      <c r="AU26" s="12"/>
+      <c r="AV26" s="12"/>
+      <c r="AW26" s="12"/>
+      <c r="AX26" s="12"/>
+      <c r="AY26" s="12"/>
+      <c r="AZ26" s="12"/>
+      <c r="BA26" s="12"/>
+      <c r="BB26" s="12"/>
+      <c r="BC26" s="12"/>
+      <c r="BD26" s="13"/>
     </row>
     <row r="27" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
-      <c r="Z27" s="24"/>
-      <c r="AA27" s="24"/>
-      <c r="AB27" s="24"/>
-      <c r="AC27" s="24"/>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="24"/>
-      <c r="AG27" s="24"/>
-      <c r="AH27" s="24"/>
-      <c r="AI27" s="24"/>
-      <c r="AJ27" s="24"/>
-      <c r="AK27" s="24"/>
-      <c r="AL27" s="24"/>
-      <c r="AM27" s="24"/>
-      <c r="AN27" s="24"/>
-      <c r="AO27" s="24"/>
-      <c r="AP27" s="24"/>
-      <c r="AQ27" s="24"/>
-      <c r="AR27" s="24"/>
-      <c r="AS27" s="24"/>
-      <c r="AT27" s="24"/>
-      <c r="AU27" s="24"/>
-      <c r="AV27" s="24"/>
-      <c r="AW27" s="24"/>
-      <c r="AX27" s="24"/>
-      <c r="AY27" s="24"/>
-      <c r="AZ27" s="24"/>
-      <c r="BA27" s="24"/>
-      <c r="BB27" s="24"/>
-      <c r="BC27" s="24"/>
-      <c r="BD27" s="25"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AD27" s="12"/>
+      <c r="AE27" s="12"/>
+      <c r="AF27" s="12"/>
+      <c r="AG27" s="12"/>
+      <c r="AH27" s="12"/>
+      <c r="AI27" s="12"/>
+      <c r="AJ27" s="12"/>
+      <c r="AK27" s="12"/>
+      <c r="AL27" s="12"/>
+      <c r="AM27" s="12"/>
+      <c r="AN27" s="12"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="12"/>
+      <c r="AQ27" s="12"/>
+      <c r="AR27" s="12"/>
+      <c r="AS27" s="12"/>
+      <c r="AT27" s="12"/>
+      <c r="AU27" s="12"/>
+      <c r="AV27" s="12"/>
+      <c r="AW27" s="12"/>
+      <c r="AX27" s="12"/>
+      <c r="AY27" s="12"/>
+      <c r="AZ27" s="12"/>
+      <c r="BA27" s="12"/>
+      <c r="BB27" s="12"/>
+      <c r="BC27" s="12"/>
+      <c r="BD27" s="13"/>
     </row>
     <row r="28" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
@@ -3703,385 +3755,379 @@
       <c r="BD48" s="10"/>
     </row>
     <row r="49" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="18"/>
+      <c r="U49" s="18"/>
+      <c r="V49" s="18"/>
+      <c r="W49" s="18"/>
+      <c r="X49" s="18"/>
+      <c r="Y49" s="18"/>
+      <c r="Z49" s="18"/>
+      <c r="AA49" s="18"/>
+      <c r="AB49" s="19"/>
+      <c r="AC49" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD49" s="18"/>
+      <c r="AE49" s="18"/>
+      <c r="AF49" s="18"/>
+      <c r="AG49" s="18"/>
+      <c r="AH49" s="18"/>
+      <c r="AI49" s="18"/>
+      <c r="AJ49" s="18"/>
+      <c r="AK49" s="18"/>
+      <c r="AL49" s="18"/>
+      <c r="AM49" s="18"/>
+      <c r="AN49" s="18"/>
+      <c r="AO49" s="18"/>
+      <c r="AP49" s="18"/>
+      <c r="AQ49" s="18"/>
+      <c r="AR49" s="18"/>
+      <c r="AS49" s="18"/>
+      <c r="AT49" s="18"/>
+      <c r="AU49" s="18"/>
+      <c r="AV49" s="18"/>
+      <c r="AW49" s="18"/>
+      <c r="AX49" s="18"/>
+      <c r="AY49" s="18"/>
+      <c r="AZ49" s="18"/>
+      <c r="BA49" s="18"/>
+      <c r="BB49" s="18"/>
+      <c r="BC49" s="18"/>
+      <c r="BD49" s="19"/>
+    </row>
+    <row r="50" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="15"/>
-      <c r="R49" s="15"/>
-      <c r="S49" s="15"/>
-      <c r="T49" s="15"/>
-      <c r="U49" s="15"/>
-      <c r="V49" s="15"/>
-      <c r="W49" s="15"/>
-      <c r="X49" s="15"/>
-      <c r="Y49" s="15"/>
-      <c r="Z49" s="15"/>
-      <c r="AA49" s="15"/>
-      <c r="AB49" s="16"/>
-      <c r="AC49" s="14" t="s">
-        <v>6</v>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="23"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="23"/>
+      <c r="Q50" s="23"/>
+      <c r="R50" s="23"/>
+      <c r="S50" s="23"/>
+      <c r="T50" s="23"/>
+      <c r="U50" s="23"/>
+      <c r="V50" s="23"/>
+      <c r="W50" s="23"/>
+      <c r="X50" s="23"/>
+      <c r="Y50" s="23"/>
+      <c r="Z50" s="23"/>
+      <c r="AA50" s="23"/>
+      <c r="AB50" s="24"/>
+      <c r="AC50" s="11" t="s">
+        <v>7</v>
       </c>
-      <c r="AD49" s="15"/>
-      <c r="AE49" s="15"/>
-      <c r="AF49" s="15"/>
-      <c r="AG49" s="15"/>
-      <c r="AH49" s="15"/>
-      <c r="AI49" s="15"/>
-      <c r="AJ49" s="15"/>
-      <c r="AK49" s="15"/>
-      <c r="AL49" s="15"/>
-      <c r="AM49" s="15"/>
-      <c r="AN49" s="15"/>
-      <c r="AO49" s="15"/>
-      <c r="AP49" s="15"/>
-      <c r="AQ49" s="15"/>
-      <c r="AR49" s="15"/>
-      <c r="AS49" s="15"/>
-      <c r="AT49" s="15"/>
-      <c r="AU49" s="15"/>
-      <c r="AV49" s="15"/>
-      <c r="AW49" s="15"/>
-      <c r="AX49" s="15"/>
-      <c r="AY49" s="15"/>
-      <c r="AZ49" s="15"/>
-      <c r="BA49" s="15"/>
-      <c r="BB49" s="15"/>
-      <c r="BC49" s="15"/>
-      <c r="BD49" s="16"/>
-    </row>
-    <row r="50" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="AD50" s="23"/>
+      <c r="AE50" s="23"/>
+      <c r="AF50" s="23"/>
+      <c r="AG50" s="23"/>
+      <c r="AH50" s="23"/>
+      <c r="AI50" s="23"/>
+      <c r="AJ50" s="23"/>
+      <c r="AK50" s="23"/>
+      <c r="AL50" s="23"/>
+      <c r="AM50" s="23"/>
+      <c r="AN50" s="23"/>
+      <c r="AO50" s="23"/>
+      <c r="AP50" s="23"/>
+      <c r="AQ50" s="23"/>
+      <c r="AR50" s="23"/>
+      <c r="AS50" s="23"/>
+      <c r="AT50" s="23"/>
+      <c r="AU50" s="23"/>
+      <c r="AV50" s="23"/>
+      <c r="AW50" s="23"/>
+      <c r="AX50" s="23"/>
+      <c r="AY50" s="23"/>
+      <c r="AZ50" s="23"/>
+      <c r="BA50" s="23"/>
+      <c r="BB50" s="23"/>
+      <c r="BC50" s="23"/>
+      <c r="BD50" s="24"/>
+    </row>
+    <row r="51" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="23"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="23"/>
+      <c r="Q51" s="23"/>
+      <c r="R51" s="23"/>
+      <c r="S51" s="23"/>
+      <c r="T51" s="23"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="23"/>
+      <c r="W51" s="23"/>
+      <c r="X51" s="23"/>
+      <c r="Y51" s="23"/>
+      <c r="Z51" s="23"/>
+      <c r="AA51" s="23"/>
+      <c r="AB51" s="24"/>
+      <c r="AC51" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD51" s="23"/>
+      <c r="AE51" s="23"/>
+      <c r="AF51" s="23"/>
+      <c r="AG51" s="23"/>
+      <c r="AH51" s="23"/>
+      <c r="AI51" s="23"/>
+      <c r="AJ51" s="23"/>
+      <c r="AK51" s="23"/>
+      <c r="AL51" s="23"/>
+      <c r="AM51" s="23"/>
+      <c r="AN51" s="23"/>
+      <c r="AO51" s="23"/>
+      <c r="AP51" s="23"/>
+      <c r="AQ51" s="23"/>
+      <c r="AR51" s="23"/>
+      <c r="AS51" s="23"/>
+      <c r="AT51" s="23"/>
+      <c r="AU51" s="23"/>
+      <c r="AV51" s="23"/>
+      <c r="AW51" s="23"/>
+      <c r="AX51" s="23"/>
+      <c r="AY51" s="23"/>
+      <c r="AZ51" s="23"/>
+      <c r="BA51" s="23"/>
+      <c r="BB51" s="23"/>
+      <c r="BC51" s="23"/>
+      <c r="BD51" s="24"/>
+    </row>
+    <row r="52" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
-      <c r="V50" s="18"/>
-      <c r="W50" s="18"/>
-      <c r="X50" s="18"/>
-      <c r="Y50" s="18"/>
-      <c r="Z50" s="18"/>
-      <c r="AA50" s="18"/>
-      <c r="AB50" s="19"/>
-      <c r="AC50" s="17" t="s">
-        <v>7</v>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+      <c r="O52" s="29"/>
+      <c r="P52" s="29"/>
+      <c r="Q52" s="29"/>
+      <c r="R52" s="29"/>
+      <c r="S52" s="29"/>
+      <c r="T52" s="29"/>
+      <c r="U52" s="29"/>
+      <c r="V52" s="29"/>
+      <c r="W52" s="29"/>
+      <c r="X52" s="29"/>
+      <c r="Y52" s="29"/>
+      <c r="Z52" s="29"/>
+      <c r="AA52" s="29"/>
+      <c r="AB52" s="30"/>
+      <c r="AC52" s="28" t="s">
+        <v>11</v>
       </c>
-      <c r="AD50" s="18"/>
-      <c r="AE50" s="18"/>
-      <c r="AF50" s="18"/>
-      <c r="AG50" s="18"/>
-      <c r="AH50" s="18"/>
-      <c r="AI50" s="18"/>
-      <c r="AJ50" s="18"/>
-      <c r="AK50" s="18"/>
-      <c r="AL50" s="18"/>
-      <c r="AM50" s="18"/>
-      <c r="AN50" s="18"/>
-      <c r="AO50" s="18"/>
-      <c r="AP50" s="18"/>
-      <c r="AQ50" s="18"/>
-      <c r="AR50" s="18"/>
-      <c r="AS50" s="18"/>
-      <c r="AT50" s="18"/>
-      <c r="AU50" s="18"/>
-      <c r="AV50" s="18"/>
-      <c r="AW50" s="18"/>
-      <c r="AX50" s="18"/>
-      <c r="AY50" s="18"/>
-      <c r="AZ50" s="18"/>
-      <c r="BA50" s="18"/>
-      <c r="BB50" s="18"/>
-      <c r="BC50" s="18"/>
-      <c r="BD50" s="19"/>
-    </row>
-    <row r="51" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>5</v>
+      <c r="AD52" s="29"/>
+      <c r="AE52" s="29"/>
+      <c r="AF52" s="29"/>
+      <c r="AG52" s="29"/>
+      <c r="AH52" s="29"/>
+      <c r="AI52" s="29"/>
+      <c r="AJ52" s="29"/>
+      <c r="AK52" s="29"/>
+      <c r="AL52" s="29"/>
+      <c r="AM52" s="29"/>
+      <c r="AN52" s="29"/>
+      <c r="AO52" s="29"/>
+      <c r="AP52" s="29"/>
+      <c r="AQ52" s="29"/>
+      <c r="AR52" s="29"/>
+      <c r="AS52" s="29"/>
+      <c r="AT52" s="29"/>
+      <c r="AU52" s="29"/>
+      <c r="AV52" s="29"/>
+      <c r="AW52" s="29"/>
+      <c r="AX52" s="29"/>
+      <c r="AY52" s="29"/>
+      <c r="AZ52" s="29"/>
+      <c r="BA52" s="29"/>
+      <c r="BB52" s="29"/>
+      <c r="BC52" s="29"/>
+      <c r="BD52" s="30"/>
+    </row>
+    <row r="53" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
+        <v>16</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18"/>
-      <c r="O51" s="18"/>
-      <c r="P51" s="18"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="18"/>
-      <c r="U51" s="18"/>
-      <c r="V51" s="18"/>
-      <c r="W51" s="18"/>
-      <c r="X51" s="18"/>
-      <c r="Y51" s="18"/>
-      <c r="Z51" s="18"/>
-      <c r="AA51" s="18"/>
-      <c r="AB51" s="19"/>
-      <c r="AC51" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD51" s="18"/>
-      <c r="AE51" s="18"/>
-      <c r="AF51" s="18"/>
-      <c r="AG51" s="18"/>
-      <c r="AH51" s="18"/>
-      <c r="AI51" s="18"/>
-      <c r="AJ51" s="18"/>
-      <c r="AK51" s="18"/>
-      <c r="AL51" s="18"/>
-      <c r="AM51" s="18"/>
-      <c r="AN51" s="18"/>
-      <c r="AO51" s="18"/>
-      <c r="AP51" s="18"/>
-      <c r="AQ51" s="18"/>
-      <c r="AR51" s="18"/>
-      <c r="AS51" s="18"/>
-      <c r="AT51" s="18"/>
-      <c r="AU51" s="18"/>
-      <c r="AV51" s="18"/>
-      <c r="AW51" s="18"/>
-      <c r="AX51" s="18"/>
-      <c r="AY51" s="18"/>
-      <c r="AZ51" s="18"/>
-      <c r="BA51" s="18"/>
-      <c r="BB51" s="18"/>
-      <c r="BC51" s="18"/>
-      <c r="BD51" s="19"/>
-    </row>
-    <row r="52" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="21"/>
+      <c r="N53" s="21"/>
+      <c r="O53" s="21"/>
+      <c r="P53" s="21"/>
+      <c r="Q53" s="21"/>
+      <c r="R53" s="21"/>
+      <c r="S53" s="21"/>
+      <c r="T53" s="21"/>
+      <c r="U53" s="21"/>
+      <c r="V53" s="21"/>
+      <c r="W53" s="21"/>
+      <c r="X53" s="21"/>
+      <c r="Y53" s="21"/>
+      <c r="Z53" s="21"/>
+      <c r="AA53" s="21"/>
+      <c r="AB53" s="21"/>
+      <c r="AC53" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
-      <c r="N52" s="21"/>
-      <c r="O52" s="21"/>
-      <c r="P52" s="21"/>
-      <c r="Q52" s="21"/>
-      <c r="R52" s="21"/>
-      <c r="S52" s="21"/>
-      <c r="T52" s="21"/>
-      <c r="U52" s="21"/>
-      <c r="V52" s="21"/>
-      <c r="W52" s="21"/>
-      <c r="X52" s="21"/>
-      <c r="Y52" s="21"/>
-      <c r="Z52" s="21"/>
-      <c r="AA52" s="21"/>
-      <c r="AB52" s="22"/>
-      <c r="AC52" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD52" s="21"/>
-      <c r="AE52" s="21"/>
-      <c r="AF52" s="21"/>
-      <c r="AG52" s="21"/>
-      <c r="AH52" s="21"/>
-      <c r="AI52" s="21"/>
-      <c r="AJ52" s="21"/>
-      <c r="AK52" s="21"/>
-      <c r="AL52" s="21"/>
-      <c r="AM52" s="21"/>
-      <c r="AN52" s="21"/>
-      <c r="AO52" s="21"/>
-      <c r="AP52" s="21"/>
-      <c r="AQ52" s="21"/>
-      <c r="AR52" s="21"/>
-      <c r="AS52" s="21"/>
-      <c r="AT52" s="21"/>
-      <c r="AU52" s="21"/>
-      <c r="AV52" s="21"/>
-      <c r="AW52" s="21"/>
-      <c r="AX52" s="21"/>
-      <c r="AY52" s="21"/>
-      <c r="AZ52" s="21"/>
-      <c r="BA52" s="21"/>
-      <c r="BB52" s="21"/>
-      <c r="BC52" s="21"/>
-      <c r="BD52" s="22"/>
-    </row>
-    <row r="53" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="AD53" s="21"/>
+      <c r="AE53" s="21"/>
+      <c r="AF53" s="21"/>
+      <c r="AG53" s="21"/>
+      <c r="AH53" s="21"/>
+      <c r="AI53" s="21"/>
+      <c r="AJ53" s="21"/>
+      <c r="AK53" s="21"/>
+      <c r="AL53" s="21"/>
+      <c r="AM53" s="21"/>
+      <c r="AN53" s="21"/>
+      <c r="AO53" s="21"/>
+      <c r="AP53" s="21"/>
+      <c r="AQ53" s="21"/>
+      <c r="AR53" s="21"/>
+      <c r="AS53" s="21"/>
+      <c r="AT53" s="21"/>
+      <c r="AU53" s="21"/>
+      <c r="AV53" s="21"/>
+      <c r="AW53" s="21"/>
+      <c r="AX53" s="21"/>
+      <c r="AY53" s="21"/>
+      <c r="AZ53" s="21"/>
+      <c r="BA53" s="21"/>
+      <c r="BB53" s="21"/>
+      <c r="BC53" s="21"/>
+      <c r="BD53" s="22"/>
+    </row>
+    <row r="54" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
-      <c r="L53" s="30"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="30"/>
-      <c r="O53" s="30"/>
-      <c r="P53" s="30"/>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
-      <c r="S53" s="30"/>
-      <c r="T53" s="30"/>
-      <c r="U53" s="30"/>
-      <c r="V53" s="30"/>
-      <c r="W53" s="30"/>
-      <c r="X53" s="30"/>
-      <c r="Y53" s="30"/>
-      <c r="Z53" s="30"/>
-      <c r="AA53" s="30"/>
-      <c r="AB53" s="30"/>
-      <c r="AC53" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD53" s="30"/>
-      <c r="AE53" s="30"/>
-      <c r="AF53" s="30"/>
-      <c r="AG53" s="30"/>
-      <c r="AH53" s="30"/>
-      <c r="AI53" s="30"/>
-      <c r="AJ53" s="30"/>
-      <c r="AK53" s="30"/>
-      <c r="AL53" s="30"/>
-      <c r="AM53" s="30"/>
-      <c r="AN53" s="30"/>
-      <c r="AO53" s="30"/>
-      <c r="AP53" s="30"/>
-      <c r="AQ53" s="30"/>
-      <c r="AR53" s="30"/>
-      <c r="AS53" s="30"/>
-      <c r="AT53" s="30"/>
-      <c r="AU53" s="30"/>
-      <c r="AV53" s="30"/>
-      <c r="AW53" s="30"/>
-      <c r="AX53" s="30"/>
-      <c r="AY53" s="30"/>
-      <c r="AZ53" s="30"/>
-      <c r="BA53" s="30"/>
-      <c r="BB53" s="30"/>
-      <c r="BC53" s="30"/>
-      <c r="BD53" s="31"/>
-    </row>
-    <row r="54" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="26"/>
+      <c r="R54" s="26"/>
+      <c r="S54" s="26"/>
+      <c r="T54" s="26"/>
+      <c r="U54" s="26"/>
+      <c r="V54" s="26"/>
+      <c r="W54" s="26"/>
+      <c r="X54" s="26"/>
+      <c r="Y54" s="26"/>
+      <c r="Z54" s="26"/>
+      <c r="AA54" s="26"/>
+      <c r="AB54" s="26"/>
+      <c r="AC54" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="12"/>
-      <c r="S54" s="12"/>
-      <c r="T54" s="12"/>
-      <c r="U54" s="12"/>
-      <c r="V54" s="12"/>
-      <c r="W54" s="12"/>
-      <c r="X54" s="12"/>
-      <c r="Y54" s="12"/>
-      <c r="Z54" s="12"/>
-      <c r="AA54" s="12"/>
-      <c r="AB54" s="12"/>
-      <c r="AC54" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD54" s="12"/>
-      <c r="AE54" s="12"/>
-      <c r="AF54" s="12"/>
-      <c r="AG54" s="12"/>
-      <c r="AH54" s="12"/>
-      <c r="AI54" s="12"/>
-      <c r="AJ54" s="12"/>
-      <c r="AK54" s="12"/>
-      <c r="AL54" s="12"/>
-      <c r="AM54" s="12"/>
-      <c r="AN54" s="12"/>
-      <c r="AO54" s="12"/>
-      <c r="AP54" s="12"/>
-      <c r="AQ54" s="12"/>
-      <c r="AR54" s="12"/>
-      <c r="AS54" s="12"/>
-      <c r="AT54" s="12"/>
-      <c r="AU54" s="12"/>
-      <c r="AV54" s="12"/>
-      <c r="AW54" s="12"/>
-      <c r="AX54" s="12"/>
-      <c r="AY54" s="12"/>
-      <c r="AZ54" s="12"/>
-      <c r="BA54" s="12"/>
-      <c r="BB54" s="12"/>
-      <c r="BC54" s="12"/>
-      <c r="BD54" s="13"/>
+      <c r="AD54" s="26"/>
+      <c r="AE54" s="26"/>
+      <c r="AF54" s="26"/>
+      <c r="AG54" s="26"/>
+      <c r="AH54" s="26"/>
+      <c r="AI54" s="26"/>
+      <c r="AJ54" s="26"/>
+      <c r="AK54" s="26"/>
+      <c r="AL54" s="26"/>
+      <c r="AM54" s="26"/>
+      <c r="AN54" s="26"/>
+      <c r="AO54" s="26"/>
+      <c r="AP54" s="26"/>
+      <c r="AQ54" s="26"/>
+      <c r="AR54" s="26"/>
+      <c r="AS54" s="26"/>
+      <c r="AT54" s="26"/>
+      <c r="AU54" s="26"/>
+      <c r="AV54" s="26"/>
+      <c r="AW54" s="26"/>
+      <c r="AX54" s="26"/>
+      <c r="AY54" s="26"/>
+      <c r="AZ54" s="26"/>
+      <c r="BA54" s="26"/>
+      <c r="BB54" s="26"/>
+      <c r="BC54" s="26"/>
+      <c r="BD54" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A26:BD26"/>
-    <mergeCell ref="A27:BD27"/>
-    <mergeCell ref="A1:BD1"/>
-    <mergeCell ref="A25:BD25"/>
-    <mergeCell ref="A2:BD2"/>
-    <mergeCell ref="A3:BD3"/>
     <mergeCell ref="A53:AB53"/>
     <mergeCell ref="AC53:BD53"/>
     <mergeCell ref="A54:AB54"/>
@@ -4094,6 +4140,12 @@
     <mergeCell ref="A50:AB50"/>
     <mergeCell ref="A51:AB51"/>
     <mergeCell ref="A52:AB52"/>
+    <mergeCell ref="A26:BD26"/>
+    <mergeCell ref="A27:BD27"/>
+    <mergeCell ref="A1:BD1"/>
+    <mergeCell ref="A25:BD25"/>
+    <mergeCell ref="A2:BD2"/>
+    <mergeCell ref="A3:BD3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>